<commit_message>
Docs para entrega 2
</commit_message>
<xml_diff>
--- a/TiemposBalanceador.xlsx
+++ b/TiemposBalanceador.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\je.molano1498\git\HospitalDeLosAndes---Backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanchaparro/Documents/2017-01/ARQUITECTURA DE SOFTWARE/Experimento 1/HospitalDeLosAndes---Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>LB</t>
   </si>
@@ -40,11 +46,14 @@
   <si>
     <t>Porcentaje de error (%)</t>
   </si>
+  <si>
+    <t>entrega 2 expreimento 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,29 +95,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -116,12 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -135,6 +141,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,9 +165,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -192,6 +204,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -217,7 +230,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -260,22 +273,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750</c:v>
+                  <c:v>750.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3000</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -287,28 +300,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>217</c:v>
+                  <c:v>217.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>421</c:v>
+                  <c:v>421.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>667</c:v>
+                  <c:v>667.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>672</c:v>
+                  <c:v>672.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2794</c:v>
+                  <c:v>2794.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4330</c:v>
+                  <c:v>4330.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8049-46AC-98F4-46E0FA6CFCE6}"/>
             </c:ext>
@@ -347,22 +360,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750</c:v>
+                  <c:v>750.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3000</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,28 +387,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>147</c:v>
+                  <c:v>147.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>273</c:v>
+                  <c:v>273.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>441</c:v>
+                  <c:v>441.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>853</c:v>
+                  <c:v>853.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3791</c:v>
+                  <c:v>3791.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8090</c:v>
+                  <c:v>8090.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8049-46AC-98F4-46E0FA6CFCE6}"/>
             </c:ext>
@@ -434,22 +447,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750</c:v>
+                  <c:v>750.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3000</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,28 +474,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>107</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>313</c:v>
+                  <c:v>313.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294</c:v>
+                  <c:v>294.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>586</c:v>
+                  <c:v>586.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2691</c:v>
+                  <c:v>2691.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5659</c:v>
+                  <c:v>5659.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8049-46AC-98F4-46E0FA6CFCE6}"/>
             </c:ext>
@@ -496,11 +509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="288131544"/>
-        <c:axId val="288131872"/>
+        <c:axId val="691828768"/>
+        <c:axId val="714706240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="288131544"/>
+        <c:axId val="691828768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,8 +568,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.45755424321959753"/>
-              <c:y val="0.77277704870224551"/>
+              <c:x val="0.457554243219598"/>
+              <c:y val="0.772777048702245"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -584,7 +597,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -622,15 +635,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288131872"/>
+        <c:crossAx val="714706240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="288131872"/>
+        <c:axId val="714706240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,6 +689,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -701,7 +715,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -739,10 +753,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288131544"/>
+        <c:crossAx val="691828768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -756,6 +770,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -781,7 +796,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -811,7 +826,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1398,7 +1413,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{990679DA-9C7C-49C8-AE44-1A4458B435D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{990679DA-9C7C-49C8-AE44-1A4458B435D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1716,308 +1731,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="I1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>250</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>217</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>147</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>500</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>421</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>273</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>750</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>667</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>441</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>1000</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>672</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>853</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>586</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>2000</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>2794</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>3791</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2691</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>3000</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>4330</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>8090</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>5659</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>250</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>500</v>
       </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>750</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>1000</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>2000</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>7.9299999999999995E-2</v>
       </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>3000</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>250</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>146</v>
       </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>500</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <v>317</v>
       </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>750</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>378</v>
       </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>1000</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>735</v>
       </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>2000</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>3248</v>
       </c>
-      <c r="C24" s="6">
-        <v>0</v>
-      </c>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>3000</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>6886</v>
       </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="13"/>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B10:D10"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>